<commit_message>
add examples for QT
</commit_message>
<xml_diff>
--- a/Qt_Request.xlsx
+++ b/Qt_Request.xlsx
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="107" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1531,7 +1531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="107" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>

</xml_diff>